<commit_message>
SSCS hearing list update
</commit_message>
<xml_diff>
--- a/src/integrationTest/resources/data/non-strategic/sscs-daily-hearing-list/sscsDailyHearingList.xlsx
+++ b/src/integrationTest/resources/data/non-strategic/sscs-daily-hearing-list/sscsDailyHearingList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/junaid.iqbal/Documents/GitHub/pip-data-management/src/integrationTest/resources/data/non-strategic/sscs-daily-hearing-list/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kian.kwa/IdeaProjects/pip-data-management/src/integrationTest/resources/data/non-strategic/sscs-daily-hearing-list/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF9F70CF-A3C8-6946-8B32-9506D3938878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCEB855C-834A-4449-8364-1C331F5C4471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1600" yWindow="780" windowWidth="27640" windowHeight="16940" xr2:uid="{60A97523-C16A-CF49-BC40-150250D81B47}"/>
+    <workbookView xWindow="48140" yWindow="-1020" windowWidth="27640" windowHeight="16940" xr2:uid="{60A97523-C16A-CF49-BC40-150250D81B47}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,18 +56,12 @@
     <t>Hearing Time</t>
   </si>
   <si>
-    <t>Panel</t>
-  </si>
-  <si>
     <t>FTA/Respondent</t>
   </si>
   <si>
     <t>Additional Information</t>
   </si>
   <si>
-    <t>Panel 1</t>
-  </si>
-  <si>
     <t>Additional information 1</t>
   </si>
   <si>
@@ -87,6 +81,14 @@
   </si>
   <si>
     <t>Directions</t>
+  </si>
+  <si>
+    <t>Tribunal</t>
+  </si>
+  <si>
+    <t>Tribunal member 1
+Tribunal member 2
+Tribunal member 3</t>
   </si>
 </sst>
 </file>
@@ -135,10 +137,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -157,9 +162,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -197,7 +202,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -303,7 +308,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -445,7 +450,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -456,7 +461,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -467,7 +472,7 @@
     <col min="4" max="4" width="11.5" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41" style="2" customWidth="1"/>
     <col min="8" max="8" width="14.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21.5" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="6" style="2"/>
@@ -493,42 +498,42 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>8</v>
-      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2" s="2">
         <v>1234567</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="I2" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PUB-3149 SSCS hearing list update (#838)
* SSCS hearing list update

* Fixed failing integration test

---------

Co-authored-by: github-actions[bot] <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/integrationTest/resources/data/non-strategic/sscs-daily-hearing-list/sscsDailyHearingList.xlsx
+++ b/src/integrationTest/resources/data/non-strategic/sscs-daily-hearing-list/sscsDailyHearingList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/junaid.iqbal/Documents/GitHub/pip-data-management/src/integrationTest/resources/data/non-strategic/sscs-daily-hearing-list/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kian.kwa/IdeaProjects/pip-data-management/src/integrationTest/resources/data/non-strategic/sscs-daily-hearing-list/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF9F70CF-A3C8-6946-8B32-9506D3938878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCEB855C-834A-4449-8364-1C331F5C4471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1600" yWindow="780" windowWidth="27640" windowHeight="16940" xr2:uid="{60A97523-C16A-CF49-BC40-150250D81B47}"/>
+    <workbookView xWindow="48140" yWindow="-1020" windowWidth="27640" windowHeight="16940" xr2:uid="{60A97523-C16A-CF49-BC40-150250D81B47}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,18 +56,12 @@
     <t>Hearing Time</t>
   </si>
   <si>
-    <t>Panel</t>
-  </si>
-  <si>
     <t>FTA/Respondent</t>
   </si>
   <si>
     <t>Additional Information</t>
   </si>
   <si>
-    <t>Panel 1</t>
-  </si>
-  <si>
     <t>Additional information 1</t>
   </si>
   <si>
@@ -87,6 +81,14 @@
   </si>
   <si>
     <t>Directions</t>
+  </si>
+  <si>
+    <t>Tribunal</t>
+  </si>
+  <si>
+    <t>Tribunal member 1
+Tribunal member 2
+Tribunal member 3</t>
   </si>
 </sst>
 </file>
@@ -135,10 +137,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -157,9 +162,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -197,7 +202,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -303,7 +308,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -445,7 +450,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -456,7 +461,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -467,7 +472,7 @@
     <col min="4" max="4" width="11.5" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41" style="2" customWidth="1"/>
     <col min="8" max="8" width="14.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21.5" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="6" style="2"/>
@@ -493,42 +498,42 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>8</v>
-      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2" s="2">
         <v>1234567</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="I2" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>